<commit_message>
check all (almost working correctly), clear filters, projects selected label add
</commit_message>
<xml_diff>
--- a/public/DIGITAL_PORTFOLIO.xlsx
+++ b/public/DIGITAL_PORTFOLIO.xlsx
@@ -50,6 +50,7 @@
 4. Имя файла (DIGITAL_PORTFOLIO.xlsx) должно оставаться неизменным
 5. Колонка “Клиент” нужна, чтобы в списке тегов названия компаний были первыми (если случайно продублировать это же название компании в колонку с тегами, 
 Программа поймет, что это один и тот же тег)
+6. Номера проектов не могут быть отрицательными, но могут иметь любое количество ведущих нулей: 1, 01, 001, …
 При возникновении вопросов обращайтесь в телеграм @vvh0ami</t>
     </r>
   </si>
@@ -238,8 +239,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="0000"/>
+    <numFmt numFmtId="166" formatCode="000"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -321,7 +324,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -336,6 +339,14 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -421,21 +432,21 @@
   </sheetPr>
   <dimension ref="A1:I300"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="60.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="29.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="102.67"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="189.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="203" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -779,847 +790,847 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="4"/>
+      <c r="A20" s="5"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="4"/>
+      <c r="A21" s="5"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="4"/>
+      <c r="A22" s="5"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="4"/>
+      <c r="A23" s="5"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="4"/>
+      <c r="A24" s="5"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="4"/>
+      <c r="A25" s="5"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="4"/>
+      <c r="A26" s="5"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="4"/>
+      <c r="A27" s="5"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="4"/>
+      <c r="A28" s="5"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="4"/>
+      <c r="A29" s="6"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="4"/>
+      <c r="A30" s="6"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="4"/>
+      <c r="A31" s="6"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="4"/>
+      <c r="A32" s="6"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="4"/>
+      <c r="A33" s="6"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="4"/>
+      <c r="A34" s="6"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="4"/>
+      <c r="A35" s="6"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="4"/>
+      <c r="A36" s="6"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="4"/>
+      <c r="A37" s="6"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="4"/>
+      <c r="A38" s="6"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="4"/>
+      <c r="A39" s="6"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="4"/>
+      <c r="A40" s="6"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="4"/>
+      <c r="A41" s="6"/>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="4"/>
+      <c r="A42" s="6"/>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="4"/>
+      <c r="A43" s="6"/>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="4"/>
+      <c r="A44" s="6"/>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="4"/>
+      <c r="A45" s="6"/>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="4"/>
+      <c r="A46" s="6"/>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="4"/>
+      <c r="A47" s="6"/>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="4"/>
+      <c r="A48" s="6"/>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="4"/>
+      <c r="A49" s="6"/>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="4"/>
+      <c r="A50" s="6"/>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="4"/>
+      <c r="A51" s="6"/>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="4"/>
+      <c r="A52" s="6"/>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="4"/>
+      <c r="A53" s="6"/>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="4"/>
+      <c r="A54" s="6"/>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="4"/>
+      <c r="A55" s="6"/>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="4"/>
+      <c r="A56" s="6"/>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="4"/>
+      <c r="A57" s="6"/>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="4"/>
+      <c r="A58" s="6"/>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="4"/>
+      <c r="A59" s="6"/>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="4"/>
+      <c r="A60" s="6"/>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="4"/>
+      <c r="A61" s="6"/>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="4"/>
+      <c r="A62" s="6"/>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="4"/>
+      <c r="A63" s="6"/>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="4"/>
+      <c r="A64" s="6"/>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="4"/>
+      <c r="A65" s="6"/>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="4"/>
+      <c r="A66" s="6"/>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="4"/>
+      <c r="A67" s="6"/>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="4"/>
+      <c r="A68" s="6"/>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="4"/>
+      <c r="A69" s="6"/>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="4"/>
+      <c r="A70" s="6"/>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="4"/>
+      <c r="A71" s="6"/>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="4"/>
+      <c r="A72" s="6"/>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="4"/>
+      <c r="A73" s="6"/>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="4"/>
+      <c r="A74" s="6"/>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="4"/>
+      <c r="A75" s="6"/>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="4"/>
+      <c r="A76" s="6"/>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="4"/>
+      <c r="A77" s="6"/>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="4"/>
+      <c r="A78" s="6"/>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="4"/>
+      <c r="A79" s="6"/>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="4"/>
+      <c r="A80" s="6"/>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="4"/>
+      <c r="A81" s="6"/>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="4"/>
+      <c r="A82" s="6"/>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="4"/>
+      <c r="A83" s="6"/>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="4"/>
+      <c r="A84" s="6"/>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="4"/>
+      <c r="A85" s="6"/>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="4"/>
+      <c r="A86" s="6"/>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="4"/>
+      <c r="A87" s="6"/>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="4"/>
+      <c r="A88" s="6"/>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="4"/>
+      <c r="A89" s="6"/>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="4"/>
+      <c r="A90" s="6"/>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="4"/>
+      <c r="A91" s="6"/>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="4"/>
+      <c r="A92" s="6"/>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="4"/>
+      <c r="A93" s="6"/>
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="4"/>
+      <c r="A94" s="6"/>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="4"/>
+      <c r="A95" s="6"/>
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="4"/>
+      <c r="A96" s="6"/>
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="4"/>
+      <c r="A97" s="6"/>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="4"/>
+      <c r="A98" s="6"/>
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="4"/>
+      <c r="A99" s="6"/>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="4"/>
+      <c r="A100" s="6"/>
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="4"/>
+      <c r="A101" s="6"/>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="4"/>
+      <c r="A102" s="6"/>
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="4"/>
+      <c r="A103" s="6"/>
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="4"/>
+      <c r="A104" s="6"/>
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="4"/>
+      <c r="A105" s="6"/>
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="4"/>
+      <c r="A106" s="6"/>
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="4"/>
+      <c r="A107" s="6"/>
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="4"/>
+      <c r="A108" s="6"/>
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="4"/>
+      <c r="A109" s="6"/>
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="4"/>
+      <c r="A110" s="6"/>
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="4"/>
+      <c r="A111" s="6"/>
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="4"/>
+      <c r="A112" s="6"/>
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="4"/>
+      <c r="A113" s="6"/>
     </row>
     <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="4"/>
+      <c r="A114" s="6"/>
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="4"/>
+      <c r="A115" s="6"/>
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="4"/>
+      <c r="A116" s="6"/>
     </row>
     <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="4"/>
+      <c r="A117" s="6"/>
     </row>
     <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="4"/>
+      <c r="A118" s="6"/>
     </row>
     <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="4"/>
+      <c r="A119" s="6"/>
     </row>
     <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A120" s="4"/>
+      <c r="A120" s="6"/>
     </row>
     <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="4"/>
+      <c r="A121" s="6"/>
     </row>
     <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="4"/>
+      <c r="A122" s="6"/>
     </row>
     <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="4"/>
+      <c r="A123" s="6"/>
     </row>
     <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="4"/>
+      <c r="A124" s="6"/>
     </row>
     <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A125" s="4"/>
+      <c r="A125" s="6"/>
     </row>
     <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A126" s="4"/>
+      <c r="A126" s="6"/>
     </row>
     <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A127" s="4"/>
+      <c r="A127" s="6"/>
     </row>
     <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A128" s="4"/>
+      <c r="A128" s="6"/>
     </row>
     <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A129" s="4"/>
+      <c r="A129" s="6"/>
     </row>
     <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A130" s="4"/>
+      <c r="A130" s="6"/>
     </row>
     <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A131" s="4"/>
+      <c r="A131" s="6"/>
     </row>
     <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A132" s="4"/>
+      <c r="A132" s="6"/>
     </row>
     <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A133" s="4"/>
+      <c r="A133" s="6"/>
     </row>
     <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A134" s="4"/>
+      <c r="A134" s="6"/>
     </row>
     <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A135" s="4"/>
+      <c r="A135" s="6"/>
     </row>
     <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A136" s="4"/>
+      <c r="A136" s="6"/>
     </row>
     <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A137" s="4"/>
+      <c r="A137" s="6"/>
     </row>
     <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A138" s="4"/>
+      <c r="A138" s="6"/>
     </row>
     <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A139" s="4"/>
+      <c r="A139" s="6"/>
     </row>
     <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A140" s="4"/>
+      <c r="A140" s="6"/>
     </row>
     <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A141" s="4"/>
+      <c r="A141" s="6"/>
     </row>
     <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A142" s="4"/>
+      <c r="A142" s="6"/>
     </row>
     <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A143" s="4"/>
+      <c r="A143" s="6"/>
     </row>
     <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A144" s="4"/>
+      <c r="A144" s="6"/>
     </row>
     <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A145" s="4"/>
+      <c r="A145" s="6"/>
     </row>
     <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A146" s="4"/>
+      <c r="A146" s="6"/>
     </row>
     <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A147" s="4"/>
+      <c r="A147" s="6"/>
     </row>
     <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A148" s="4"/>
+      <c r="A148" s="6"/>
     </row>
     <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A149" s="4"/>
+      <c r="A149" s="6"/>
     </row>
     <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A150" s="4"/>
+      <c r="A150" s="6"/>
     </row>
     <row r="151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A151" s="4"/>
+      <c r="A151" s="6"/>
     </row>
     <row r="152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A152" s="4"/>
+      <c r="A152" s="6"/>
     </row>
     <row r="153" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A153" s="4"/>
+      <c r="A153" s="6"/>
     </row>
     <row r="154" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A154" s="4"/>
+      <c r="A154" s="6"/>
     </row>
     <row r="155" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A155" s="4"/>
+      <c r="A155" s="6"/>
     </row>
     <row r="156" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A156" s="4"/>
+      <c r="A156" s="6"/>
     </row>
     <row r="157" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A157" s="4"/>
+      <c r="A157" s="6"/>
     </row>
     <row r="158" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A158" s="4"/>
+      <c r="A158" s="6"/>
     </row>
     <row r="159" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A159" s="4"/>
+      <c r="A159" s="6"/>
     </row>
     <row r="160" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A160" s="4"/>
+      <c r="A160" s="6"/>
     </row>
     <row r="161" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A161" s="4"/>
+      <c r="A161" s="6"/>
     </row>
     <row r="162" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A162" s="4"/>
+      <c r="A162" s="6"/>
     </row>
     <row r="163" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A163" s="4"/>
+      <c r="A163" s="6"/>
     </row>
     <row r="164" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A164" s="4"/>
+      <c r="A164" s="6"/>
     </row>
     <row r="165" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A165" s="4"/>
+      <c r="A165" s="6"/>
     </row>
     <row r="166" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A166" s="4"/>
+      <c r="A166" s="6"/>
     </row>
     <row r="167" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A167" s="4"/>
+      <c r="A167" s="6"/>
     </row>
     <row r="168" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A168" s="4"/>
+      <c r="A168" s="6"/>
     </row>
     <row r="169" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A169" s="4"/>
+      <c r="A169" s="6"/>
     </row>
     <row r="170" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A170" s="4"/>
+      <c r="A170" s="6"/>
     </row>
     <row r="171" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A171" s="4"/>
+      <c r="A171" s="6"/>
     </row>
     <row r="172" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A172" s="4"/>
+      <c r="A172" s="6"/>
     </row>
     <row r="173" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A173" s="4"/>
+      <c r="A173" s="6"/>
     </row>
     <row r="174" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A174" s="4"/>
+      <c r="A174" s="6"/>
     </row>
     <row r="175" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A175" s="4"/>
+      <c r="A175" s="6"/>
     </row>
     <row r="176" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A176" s="4"/>
+      <c r="A176" s="6"/>
     </row>
     <row r="177" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A177" s="4"/>
+      <c r="A177" s="6"/>
     </row>
     <row r="178" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A178" s="4"/>
+      <c r="A178" s="6"/>
     </row>
     <row r="179" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A179" s="4"/>
+      <c r="A179" s="6"/>
     </row>
     <row r="180" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A180" s="4"/>
+      <c r="A180" s="6"/>
     </row>
     <row r="181" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A181" s="4"/>
+      <c r="A181" s="6"/>
     </row>
     <row r="182" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A182" s="4"/>
+      <c r="A182" s="6"/>
     </row>
     <row r="183" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A183" s="4"/>
+      <c r="A183" s="6"/>
     </row>
     <row r="184" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A184" s="4"/>
+      <c r="A184" s="6"/>
     </row>
     <row r="185" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A185" s="4"/>
+      <c r="A185" s="6"/>
     </row>
     <row r="186" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A186" s="4"/>
+      <c r="A186" s="6"/>
     </row>
     <row r="187" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A187" s="4"/>
+      <c r="A187" s="6"/>
     </row>
     <row r="188" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A188" s="4"/>
+      <c r="A188" s="6"/>
     </row>
     <row r="189" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A189" s="4"/>
+      <c r="A189" s="6"/>
     </row>
     <row r="190" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A190" s="4"/>
+      <c r="A190" s="6"/>
     </row>
     <row r="191" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A191" s="4"/>
+      <c r="A191" s="6"/>
     </row>
     <row r="192" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A192" s="4"/>
+      <c r="A192" s="6"/>
     </row>
     <row r="193" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A193" s="4"/>
+      <c r="A193" s="6"/>
     </row>
     <row r="194" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A194" s="4"/>
+      <c r="A194" s="6"/>
     </row>
     <row r="195" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A195" s="4"/>
+      <c r="A195" s="6"/>
     </row>
     <row r="196" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A196" s="4"/>
+      <c r="A196" s="6"/>
     </row>
     <row r="197" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A197" s="4"/>
+      <c r="A197" s="6"/>
     </row>
     <row r="198" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A198" s="4"/>
+      <c r="A198" s="6"/>
     </row>
     <row r="199" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A199" s="4"/>
+      <c r="A199" s="6"/>
     </row>
     <row r="200" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A200" s="4"/>
+      <c r="A200" s="6"/>
     </row>
     <row r="201" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A201" s="4"/>
+      <c r="A201" s="6"/>
     </row>
     <row r="202" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A202" s="4"/>
+      <c r="A202" s="6"/>
     </row>
     <row r="203" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A203" s="4"/>
+      <c r="A203" s="6"/>
     </row>
     <row r="204" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A204" s="4"/>
+      <c r="A204" s="6"/>
     </row>
     <row r="205" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A205" s="4"/>
+      <c r="A205" s="6"/>
     </row>
     <row r="206" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A206" s="4"/>
+      <c r="A206" s="6"/>
     </row>
     <row r="207" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A207" s="4"/>
+      <c r="A207" s="6"/>
     </row>
     <row r="208" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A208" s="4"/>
+      <c r="A208" s="6"/>
     </row>
     <row r="209" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A209" s="4"/>
+      <c r="A209" s="6"/>
     </row>
     <row r="210" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A210" s="4"/>
+      <c r="A210" s="6"/>
     </row>
     <row r="211" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A211" s="4"/>
+      <c r="A211" s="6"/>
     </row>
     <row r="212" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A212" s="4"/>
+      <c r="A212" s="6"/>
     </row>
     <row r="213" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A213" s="4"/>
+      <c r="A213" s="6"/>
     </row>
     <row r="214" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A214" s="4"/>
+      <c r="A214" s="6"/>
     </row>
     <row r="215" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A215" s="4"/>
+      <c r="A215" s="6"/>
     </row>
     <row r="216" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A216" s="4"/>
+      <c r="A216" s="6"/>
     </row>
     <row r="217" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A217" s="4"/>
+      <c r="A217" s="6"/>
     </row>
     <row r="218" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A218" s="4"/>
+      <c r="A218" s="6"/>
     </row>
     <row r="219" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A219" s="4"/>
+      <c r="A219" s="6"/>
     </row>
     <row r="220" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A220" s="4"/>
+      <c r="A220" s="6"/>
     </row>
     <row r="221" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A221" s="4"/>
+      <c r="A221" s="6"/>
     </row>
     <row r="222" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A222" s="4"/>
+      <c r="A222" s="6"/>
     </row>
     <row r="223" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A223" s="4"/>
+      <c r="A223" s="6"/>
     </row>
     <row r="224" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A224" s="4"/>
+      <c r="A224" s="6"/>
     </row>
     <row r="225" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A225" s="4"/>
+      <c r="A225" s="6"/>
     </row>
     <row r="226" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A226" s="4"/>
+      <c r="A226" s="6"/>
     </row>
     <row r="227" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A227" s="4"/>
+      <c r="A227" s="6"/>
     </row>
     <row r="228" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A228" s="4"/>
+      <c r="A228" s="6"/>
     </row>
     <row r="229" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A229" s="4"/>
+      <c r="A229" s="6"/>
     </row>
     <row r="230" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A230" s="4"/>
+      <c r="A230" s="6"/>
     </row>
     <row r="231" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A231" s="4"/>
+      <c r="A231" s="6"/>
     </row>
     <row r="232" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A232" s="4"/>
+      <c r="A232" s="6"/>
     </row>
     <row r="233" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A233" s="4"/>
+      <c r="A233" s="6"/>
     </row>
     <row r="234" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A234" s="4"/>
+      <c r="A234" s="6"/>
     </row>
     <row r="235" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A235" s="4"/>
+      <c r="A235" s="6"/>
     </row>
     <row r="236" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A236" s="4"/>
+      <c r="A236" s="6"/>
     </row>
     <row r="237" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A237" s="4"/>
+      <c r="A237" s="6"/>
     </row>
     <row r="238" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A238" s="4"/>
+      <c r="A238" s="6"/>
     </row>
     <row r="239" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A239" s="4"/>
+      <c r="A239" s="6"/>
     </row>
     <row r="240" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A240" s="4"/>
+      <c r="A240" s="6"/>
     </row>
     <row r="241" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A241" s="4"/>
+      <c r="A241" s="6"/>
     </row>
     <row r="242" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A242" s="4"/>
+      <c r="A242" s="6"/>
     </row>
     <row r="243" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A243" s="4"/>
+      <c r="A243" s="6"/>
     </row>
     <row r="244" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A244" s="4"/>
+      <c r="A244" s="6"/>
     </row>
     <row r="245" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A245" s="4"/>
+      <c r="A245" s="6"/>
     </row>
     <row r="246" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A246" s="4"/>
+      <c r="A246" s="6"/>
     </row>
     <row r="247" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A247" s="4"/>
+      <c r="A247" s="6"/>
     </row>
     <row r="248" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A248" s="4"/>
+      <c r="A248" s="6"/>
     </row>
     <row r="249" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A249" s="4"/>
+      <c r="A249" s="6"/>
     </row>
     <row r="250" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A250" s="4"/>
+      <c r="A250" s="6"/>
     </row>
     <row r="251" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A251" s="4"/>
+      <c r="A251" s="6"/>
     </row>
     <row r="252" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A252" s="4"/>
+      <c r="A252" s="6"/>
     </row>
     <row r="253" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A253" s="4"/>
+      <c r="A253" s="6"/>
     </row>
     <row r="254" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A254" s="4"/>
+      <c r="A254" s="6"/>
     </row>
     <row r="255" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A255" s="4"/>
+      <c r="A255" s="6"/>
     </row>
     <row r="256" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A256" s="4"/>
+      <c r="A256" s="6"/>
     </row>
     <row r="257" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A257" s="4"/>
+      <c r="A257" s="6"/>
     </row>
     <row r="258" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A258" s="4"/>
+      <c r="A258" s="6"/>
     </row>
     <row r="259" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A259" s="4"/>
+      <c r="A259" s="6"/>
     </row>
     <row r="260" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A260" s="4"/>
+      <c r="A260" s="6"/>
     </row>
     <row r="261" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A261" s="4"/>
+      <c r="A261" s="6"/>
     </row>
     <row r="262" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A262" s="4"/>
+      <c r="A262" s="6"/>
     </row>
     <row r="263" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A263" s="4"/>
+      <c r="A263" s="6"/>
     </row>
     <row r="264" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A264" s="4"/>
+      <c r="A264" s="6"/>
     </row>
     <row r="265" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A265" s="4"/>
+      <c r="A265" s="6"/>
     </row>
     <row r="266" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A266" s="4"/>
+      <c r="A266" s="6"/>
     </row>
     <row r="267" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A267" s="4"/>
+      <c r="A267" s="6"/>
     </row>
     <row r="268" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A268" s="4"/>
+      <c r="A268" s="6"/>
     </row>
     <row r="269" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A269" s="4"/>
+      <c r="A269" s="6"/>
     </row>
     <row r="270" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A270" s="4"/>
+      <c r="A270" s="6"/>
     </row>
     <row r="271" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A271" s="4"/>
+      <c r="A271" s="6"/>
     </row>
     <row r="272" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A272" s="4"/>
+      <c r="A272" s="6"/>
     </row>
     <row r="273" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A273" s="4"/>
+      <c r="A273" s="6"/>
     </row>
     <row r="274" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A274" s="4"/>
+      <c r="A274" s="6"/>
     </row>
     <row r="275" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A275" s="4"/>
+      <c r="A275" s="6"/>
     </row>
     <row r="276" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A276" s="4"/>
+      <c r="A276" s="6"/>
     </row>
     <row r="277" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A277" s="4"/>
+      <c r="A277" s="6"/>
     </row>
     <row r="278" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A278" s="4"/>
+      <c r="A278" s="6"/>
     </row>
     <row r="279" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A279" s="4"/>
+      <c r="A279" s="6"/>
     </row>
     <row r="280" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A280" s="4"/>
+      <c r="A280" s="6"/>
     </row>
     <row r="281" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A281" s="4"/>
+      <c r="A281" s="6"/>
     </row>
     <row r="282" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A282" s="4"/>
+      <c r="A282" s="6"/>
     </row>
     <row r="283" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A283" s="4"/>
+      <c r="A283" s="6"/>
     </row>
     <row r="284" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A284" s="4"/>
+      <c r="A284" s="6"/>
     </row>
     <row r="285" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A285" s="4"/>
+      <c r="A285" s="6"/>
     </row>
     <row r="286" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A286" s="4"/>
+      <c r="A286" s="6"/>
     </row>
     <row r="287" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A287" s="4"/>
+      <c r="A287" s="6"/>
     </row>
     <row r="288" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A288" s="4"/>
+      <c r="A288" s="6"/>
     </row>
     <row r="289" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A289" s="4"/>
+      <c r="A289" s="6"/>
     </row>
     <row r="290" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A290" s="4"/>
+      <c r="A290" s="6"/>
     </row>
     <row r="291" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A291" s="4"/>
+      <c r="A291" s="6"/>
     </row>
     <row r="292" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A292" s="4"/>
+      <c r="A292" s="6"/>
     </row>
     <row r="293" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A293" s="4"/>
+      <c r="A293" s="6"/>
     </row>
     <row r="294" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A294" s="4"/>
+      <c r="A294" s="6"/>
     </row>
     <row r="295" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A295" s="4"/>
+      <c r="A295" s="6"/>
     </row>
     <row r="296" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A296" s="4"/>
+      <c r="A296" s="6"/>
     </row>
     <row r="297" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A297" s="4"/>
+      <c r="A297" s="6"/>
     </row>
     <row r="298" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A298" s="4"/>
+      <c r="A298" s="6"/>
     </row>
     <row r="299" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A299" s="4"/>
+      <c r="A299" s="6"/>
     </row>
     <row r="300" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A300" s="4"/>
+      <c r="A300" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
add dnd cards at page 2
</commit_message>
<xml_diff>
--- a/public/DIGITAL_PORTFOLIO.xlsx
+++ b/public/DIGITAL_PORTFOLIO.xlsx
@@ -46,12 +46,29 @@
 1. Новая строка – новый проект
 2. Названия колонок (желтые) нельзя переименовывать или переставлять местами 
 2. Когда в ячейку нужно вписать несколько значений (имена файлов, категории), вписывайте их через запятую с пробелом
-3. Теги нужно писать везде одинаково (например, нельзя в одном проекте написать “фирменный стиль”, а в другом “Фирменный стиль”, это будут 2 разных тега для программы
-4. Имя файла (DIGITAL_PORTFOLIO.xlsx) должно оставаться неизменным
-5. Колонка “Клиент” нужна, чтобы в списке тегов названия компаний были первыми (если случайно продублировать это же название компании в колонку с тегами, 
-Программа поймет, что это один и тот же тег)
-6. Номера проектов не могут быть отрицательными, но могут иметь любое количество ведущих нулей: 1, 01, 001, …
-При возникновении вопросов обращайтесь в телеграм @vvh0ami</t>
+3. Теги нужно писать везде одинаково (например, нельзя в одном проекте написать “фирменный стиль”, а в другом “Фирменный стиль”, это будут 2 разных тега для программы)
+4. Номера проектов  могут иметь любое количество ведущих нулей: 1, 01, 001, … (не могут быть отрицательными)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">5. Имя файла (DIGITAL_PORTFOLIO.xlsx) должно оставаться неизменным
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">При возникновении вопросов обращайтесь в телеграм @vvh0ami</t>
     </r>
   </si>
   <si>
@@ -244,7 +261,7 @@
     <numFmt numFmtId="165" formatCode="0000"/>
     <numFmt numFmtId="166" formatCode="000"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -274,6 +291,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -436,7 +459,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.67"/>

</xml_diff>

<commit_message>
add pdf generation, bug: page always refreshes after fetch
</commit_message>
<xml_diff>
--- a/public/DIGITAL_PORTFOLIO.xlsx
+++ b/public/DIGITAL_PORTFOLIO.xlsx
@@ -43,11 +43,10 @@
         <charset val="204"/>
       </rPr>
       <t xml:space="preserve">Программа для генерации портфолио берёт информацию из этой таблицы, так что при её редактировании нужно обязательно соблюдать следующий формат:
-1. Новая строка – новый проект
-2. Названия колонок (желтые) нельзя переименовывать или переставлять местами 
+1. Названия колонок (желтые) нельзя переименовывать или переставлять местами 
 2. Когда в ячейку нужно вписать несколько значений (имена файлов, категории), вписывайте их через запятую с пробелом
 3. Теги нужно писать везде одинаково (например, нельзя в одном проекте написать “фирменный стиль”, а в другом “Фирменный стиль”, это будут 2 разных тега для программы)
-4. Номера проектов  могут иметь любое количество ведущих нулей: 1, 01, 001, … (не могут быть отрицательными)
+4. Номера проектов  могут иметь любое количество ведущих нулей: 1, 01, 001, …
 </t>
     </r>
     <r>
@@ -56,8 +55,9 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">5. Имя файла (DIGITAL_PORTFOLIO.xlsx) должно оставаться неизменным
+      <t xml:space="preserve">5. Имя этого файла (DIGITAL_PORTFOLIO.xlsx) должно оставаться неизменным
 </t>
     </r>
     <r>
@@ -297,6 +297,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -456,10 +457,10 @@
   <dimension ref="A1:I300"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.67"/>

</xml_diff>

<commit_message>
fix loading icon, add json-near-to-pdf feature
</commit_message>
<xml_diff>
--- a/public/DIGITAL_PORTFOLIO.xlsx
+++ b/public/DIGITAL_PORTFOLIO.xlsx
@@ -47,6 +47,7 @@
 2. Когда в ячейку нужно вписать несколько значений (имена файлов, категории), вписывайте их через запятую с пробелом
 3. Теги нужно писать везде одинаково (например, нельзя в одном проекте написать “фирменный стиль”, а в другом “Фирменный стиль”, это будут 2 разных тега для программы)
 4. Номера проектов  могут иметь любое количество ведущих нулей: 1, 01, 001, …
+5. Нельзя менять номер проекта, иметь два проекта с одинаковым номером (но если что, программа скажет об этом)
 </t>
     </r>
     <r>
@@ -57,7 +58,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">5. Имя этого файла (DIGITAL_PORTFOLIO.xlsx) должно оставаться неизменным
+      <t xml:space="preserve">6. Имя этого файла (DIGITAL_PORTFOLIO.xlsx) должно оставаться неизменным
 </t>
     </r>
     <r>
@@ -457,10 +458,10 @@
   <dimension ref="A1:I300"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.67"/>

</xml_diff>

<commit_message>
add project system, that works great (except files sorting and possibility to name the portfolios)
</commit_message>
<xml_diff>
--- a/public/DIGITAL_PORTFOLIO.xlsx
+++ b/public/DIGITAL_PORTFOLIO.xlsx
@@ -457,11 +457,11 @@
   </sheetPr>
   <dimension ref="A1:I300"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M47" activeCellId="0" sqref="M47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.41015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.67"/>

</xml_diff>